<commit_message>
fix edit logic of card
</commit_message>
<xml_diff>
--- a/Usecase.xlsx
+++ b/Usecase.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="131">
   <si>
     <t>Localstorage</t>
   </si>
@@ -59,7 +59,7 @@
     <t>hh:mm</t>
   </si>
   <si>
-    <t>allNotes</t>
+    <t>notes</t>
   </si>
   <si>
     <t>{ [dd/mm/yyyy]: Note[] }</t>
@@ -116,6 +116,9 @@
     <t>Main panel</t>
   </si>
   <si>
+    <t>DayCard</t>
+  </si>
+  <si>
     <t>Calendar</t>
   </si>
   <si>
@@ -125,6 +128,12 @@
     <t>Can config how many days in week view</t>
   </si>
   <si>
+    <t>LeftClick on Num</t>
+  </si>
+  <si>
+    <t>→ Switch view to day and set day</t>
+  </si>
+  <si>
     <t>Mark current day</t>
   </si>
   <si>
@@ -149,7 +158,10 @@
     <t>Daytab</t>
   </si>
   <si>
-    <t>DayCard</t>
+    <t>Dragover body</t>
+  </si>
+  <si>
+    <t>→ Show all full empty zone</t>
   </si>
   <si>
     <t>Double click on day to go to selected day</t>
@@ -167,64 +179,55 @@
     <t>tap new note zone</t>
   </si>
   <si>
+    <t>Merge all task</t>
+  </si>
+  <si>
+    <t>→ Task will be fill to drop date</t>
+  </si>
+  <si>
+    <t>left drag a day</t>
+  </si>
+  <si>
+    <t>hold → drag → merge/switch dialog</t>
+  </si>
+  <si>
+    <t>Planing</t>
+  </si>
+  <si>
+    <t>Switch all task</t>
+  </si>
+  <si>
+    <t>→ Task will be switched between dates</t>
+  </si>
+  <si>
+    <t>right drag a day</t>
+  </si>
+  <si>
+    <t>Contain notes as a normal day tab view</t>
+  </si>
+  <si>
+    <t>Open all actions</t>
+  </si>
+  <si>
+    <t>right click</t>
+  </si>
+  <si>
+    <t>Noting a day</t>
+  </si>
+  <si>
+    <t>→ Display above all notes</t>
+  </si>
+  <si>
+    <t>NoteCard</t>
+  </si>
+  <si>
+    <t>Mark a day</t>
+  </si>
+  <si>
+    <t>→ Display as important</t>
+  </si>
+  <si>
     <t>LeftClick</t>
-  </si>
-  <si>
-    <t>→ Switch view to day and set day</t>
-  </si>
-  <si>
-    <t>Merge all task</t>
-  </si>
-  <si>
-    <t>→ Task will be fill to drop date</t>
-  </si>
-  <si>
-    <t>left drag a day</t>
-  </si>
-  <si>
-    <t>hold → drag → merge/switch dialog</t>
-  </si>
-  <si>
-    <t>Dragover</t>
-  </si>
-  <si>
-    <t>→ Show all full empty zone</t>
-  </si>
-  <si>
-    <t>Planing</t>
-  </si>
-  <si>
-    <t>Switch all task</t>
-  </si>
-  <si>
-    <t>→ Task will be switched between dates</t>
-  </si>
-  <si>
-    <t>right drag a day</t>
-  </si>
-  <si>
-    <t>Contain notes as a normal day tab view</t>
-  </si>
-  <si>
-    <t>Open all actions</t>
-  </si>
-  <si>
-    <t>right click</t>
-  </si>
-  <si>
-    <t>Noting a day</t>
-  </si>
-  <si>
-    <t>→ Display above all notes</t>
-  </si>
-  <si>
-    <t>NoteCard</t>
-  </si>
-  <si>
-    <t>Mark a day</t>
-  </si>
-  <si>
-    <t>→ Display as important</t>
   </si>
   <si>
     <t>→ Select</t>
@@ -412,7 +415,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,19 +461,6 @@
       <i/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Bellota"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Bellota"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Bellota"/>
       <family val="2"/>
     </font>
@@ -564,6 +554,9 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -572,6 +565,9 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -613,12 +609,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="17" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -929,51 +919,51 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="5" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="5" width="21.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="5" width="21.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="5" width="21.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="5" width="21.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="5" width="29.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="5" width="3.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="5" width="4.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="5" width="10.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="5" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="5" width="10.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="5" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="9.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="6" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="6" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="6" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="6" width="21.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="6" width="21.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="6" width="21.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="6" width="21.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="6" width="29.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="6" width="3.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="6" width="4.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="6" width="10.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="6" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="6" width="24.005" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="2"/>
@@ -983,8 +973,8 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="2"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="3"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -1019,31 +1009,31 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="2"/>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="7" t="s">
+      <c r="I2" s="9"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="9" t="s">
         <v>28</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="9" t="s">
         <v>29</v>
       </c>
       <c r="O2" s="2"/>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="9" t="s">
         <v>30</v>
       </c>
       <c r="Q2" s="2"/>
@@ -1073,7 +1063,7 @@
       <c r="AO2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="8"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1082,17 +1072,17 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="J3" s="3"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
-      <c r="T3" s="10"/>
+      <c r="T3" s="12"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
@@ -1106,17 +1096,17 @@
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
-      <c r="AH3" s="11"/>
-      <c r="AI3" s="12"/>
+      <c r="AH3" s="13"/>
+      <c r="AI3" s="14"/>
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
       <c r="AL3" s="2"/>
       <c r="AM3" s="2"/>
-      <c r="AN3" s="11"/>
-      <c r="AO3" s="12"/>
+      <c r="AN3" s="13"/>
+      <c r="AO3" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="2"/>
@@ -1126,8 +1116,8 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="7" t="s">
+      <c r="I4" s="15"/>
+      <c r="J4" s="9" t="s">
         <v>32</v>
       </c>
       <c r="K4" s="2"/>
@@ -1137,12 +1127,14 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="6"/>
+      <c r="R4" s="8"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
+      <c r="W4" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
@@ -1163,9 +1155,9 @@
       <c r="AO4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7" t="s">
-        <v>33</v>
+      <c r="A5" s="8"/>
+      <c r="B5" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1174,26 +1166,30 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="6" t="s">
-        <v>34</v>
+      <c r="J5" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="7" t="s">
-        <v>35</v>
+      <c r="M5" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-      <c r="S5" s="6"/>
+      <c r="S5" s="8"/>
       <c r="T5" s="2"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
+      <c r="Y5" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
@@ -1214,8 +1210,8 @@
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="7" t="s">
-        <v>36</v>
+      <c r="C6" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1223,30 +1219,32 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="6" t="s">
-        <v>37</v>
+      <c r="J6" s="3"/>
+      <c r="K6" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q6" s="7" t="s">
+      <c r="N6" s="9" t="s">
         <v>41</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
+      <c r="W6" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
@@ -1269,8 +1267,8 @@
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="7" t="s">
-        <v>42</v>
+      <c r="C7" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1278,9 +1276,9 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="6" t="s">
-        <v>43</v>
+      <c r="J7" s="3"/>
+      <c r="K7" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -1289,15 +1287,17 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="6"/>
+      <c r="S7" s="8"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
-      <c r="W7" s="6" t="s">
-        <v>44</v>
+      <c r="W7" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
+      <c r="Y7" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
@@ -1318,8 +1318,8 @@
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="7" t="s">
-        <v>45</v>
+      <c r="C8" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1327,34 +1327,30 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="6"/>
+      <c r="J8" s="8"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="7" t="s">
-        <v>46</v>
+      <c r="L8" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="M8" s="2"/>
-      <c r="N8" s="7" t="s">
-        <v>47</v>
+      <c r="N8" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="O8" s="2"/>
-      <c r="P8" s="15" t="s">
-        <v>48</v>
+      <c r="P8" s="17" t="s">
+        <v>52</v>
       </c>
       <c r="Q8" s="2"/>
-      <c r="R8" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="S8" s="6"/>
+      <c r="R8" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="S8" s="8"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
-      <c r="W8" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="W8" s="2"/>
       <c r="X8" s="2"/>
-      <c r="Y8" s="7" t="s">
-        <v>51</v>
-      </c>
+      <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
@@ -1382,34 +1378,30 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="J9" s="3"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="7" t="s">
-        <v>52</v>
+      <c r="L9" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="M9" s="2"/>
-      <c r="N9" s="7" t="s">
-        <v>53</v>
+      <c r="N9" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="O9" s="2"/>
-      <c r="P9" s="15" t="s">
-        <v>54</v>
+      <c r="P9" s="17" t="s">
+        <v>56</v>
       </c>
       <c r="Q9" s="2"/>
-      <c r="R9" s="16" t="s">
-        <v>55</v>
+      <c r="R9" s="18" t="s">
+        <v>57</v>
       </c>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
-      <c r="W9" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="W9" s="2"/>
       <c r="X9" s="2"/>
-      <c r="Y9" s="7" t="s">
-        <v>57</v>
-      </c>
+      <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
@@ -1429,7 +1421,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="2"/>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="9" t="s">
         <v>58</v>
       </c>
       <c r="C10" s="2"/>
@@ -1439,21 +1431,21 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="J10" s="3"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="9" t="s">
         <v>59</v>
       </c>
       <c r="M10" s="2"/>
-      <c r="N10" s="7" t="s">
+      <c r="N10" s="9" t="s">
         <v>60</v>
       </c>
       <c r="O10" s="2"/>
-      <c r="P10" s="15" t="s">
+      <c r="P10" s="17" t="s">
         <v>61</v>
       </c>
       <c r="Q10" s="2"/>
-      <c r="R10" s="17"/>
+      <c r="R10" s="19"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
@@ -1481,7 +1473,7 @@
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="9" t="s">
         <v>62</v>
       </c>
       <c r="D11" s="2"/>
@@ -1490,15 +1482,15 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="J11" s="3"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="8" t="s">
         <v>63</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
-      <c r="P11" s="7" t="s">
+      <c r="P11" s="9" t="s">
         <v>64</v>
       </c>
       <c r="Q11" s="2"/>
@@ -1537,13 +1529,13 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="J12" s="3"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="7" t="s">
+      <c r="M12" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="N12" s="7" t="s">
+      <c r="N12" s="9" t="s">
         <v>66</v>
       </c>
       <c r="O12" s="2"/>
@@ -1554,7 +1546,7 @@
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
-      <c r="W12" s="6" t="s">
+      <c r="W12" s="8" t="s">
         <v>67</v>
       </c>
       <c r="X12" s="2"/>
@@ -1586,13 +1578,13 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="J13" s="3"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="7" t="s">
+      <c r="M13" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="N13" s="7" t="s">
+      <c r="N13" s="9" t="s">
         <v>69</v>
       </c>
       <c r="O13" s="2"/>
@@ -1603,12 +1595,12 @@
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
-      <c r="W13" s="7" t="s">
-        <v>50</v>
+      <c r="W13" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="X13" s="2"/>
-      <c r="Y13" s="7" t="s">
-        <v>70</v>
+      <c r="Y13" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
@@ -1637,14 +1629,14 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="J14" s="3"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="6" t="s">
-        <v>71</v>
+      <c r="L14" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="M14" s="2"/>
-      <c r="N14" s="7" t="s">
-        <v>72</v>
+      <c r="N14" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
@@ -1654,20 +1646,20 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
-      <c r="W14" s="7" t="s">
-        <v>73</v>
+      <c r="W14" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="X14" s="2"/>
-      <c r="Y14" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z14" s="7" t="s">
+      <c r="Y14" s="9" t="s">
         <v>75</v>
+      </c>
+      <c r="Z14" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
-      <c r="AC14" s="7" t="s">
-        <v>76</v>
+      <c r="AC14" s="9" t="s">
+        <v>77</v>
       </c>
       <c r="AD14" s="2"/>
       <c r="AE14" s="2"/>
@@ -1692,7 +1684,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="J15" s="3"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -1705,12 +1697,12 @@
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
-      <c r="W15" s="7" t="s">
-        <v>77</v>
+      <c r="W15" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="X15" s="2"/>
-      <c r="Y15" s="7" t="s">
-        <v>78</v>
+      <c r="Y15" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
@@ -1739,11 +1731,11 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="6" t="s">
+      <c r="J16" s="3"/>
+      <c r="K16" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="L16" s="7"/>
+      <c r="L16" s="9"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -1754,12 +1746,12 @@
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
-      <c r="W16" s="7" t="s">
-        <v>79</v>
+      <c r="W16" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="X16" s="2"/>
-      <c r="Y16" s="7" t="s">
-        <v>80</v>
+      <c r="Y16" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
@@ -1788,17 +1780,17 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="6" t="s">
-        <v>81</v>
+      <c r="J17" s="3"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="M17" s="2"/>
-      <c r="N17" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="O17" s="7" t="s">
+      <c r="N17" s="9" t="s">
         <v>83</v>
+      </c>
+      <c r="O17" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
@@ -1807,12 +1799,12 @@
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
-      <c r="W17" s="7" t="s">
-        <v>84</v>
+      <c r="W17" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="X17" s="2"/>
-      <c r="Y17" s="7" t="s">
-        <v>85</v>
+      <c r="Y17" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
@@ -1841,27 +1833,27 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="7"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="9"/>
       <c r="M18" s="2"/>
-      <c r="N18" s="7" t="s">
-        <v>86</v>
+      <c r="N18" s="9" t="s">
+        <v>87</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
-      <c r="R18" s="6"/>
+      <c r="R18" s="8"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
-      <c r="W18" s="7" t="s">
-        <v>87</v>
+      <c r="W18" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="X18" s="2"/>
-      <c r="Y18" s="7" t="s">
-        <v>88</v>
+      <c r="Y18" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
@@ -1890,9 +1882,9 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="7"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="9"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -1933,9 +1925,9 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="7"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="9"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -1946,12 +1938,12 @@
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
-      <c r="W20" s="7" t="s">
-        <v>89</v>
+      <c r="W20" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="X20" s="2"/>
-      <c r="Y20" s="7" t="s">
-        <v>90</v>
+      <c r="Y20" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
@@ -1980,9 +1972,9 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="7"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="9"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -2023,21 +2015,21 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="6" t="s">
-        <v>91</v>
+      <c r="J22" s="3"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="M22" s="2"/>
-      <c r="N22" s="7" t="s">
-        <v>92</v>
+      <c r="N22" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="O22" s="2"/>
-      <c r="P22" s="15" t="s">
-        <v>93</v>
+      <c r="P22" s="17" t="s">
+        <v>94</v>
       </c>
       <c r="Q22" s="2"/>
-      <c r="R22" s="15"/>
+      <c r="R22" s="17"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
@@ -2072,19 +2064,19 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="7"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="9"/>
       <c r="M23" s="2"/>
-      <c r="N23" s="7" t="s">
-        <v>94</v>
+      <c r="N23" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="O23" s="2"/>
-      <c r="P23" s="15" t="s">
-        <v>95</v>
+      <c r="P23" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="Q23" s="2"/>
-      <c r="R23" s="15"/>
+      <c r="R23" s="17"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
@@ -2119,19 +2111,19 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="7"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="9"/>
       <c r="M24" s="2"/>
-      <c r="N24" s="7" t="s">
-        <v>96</v>
+      <c r="N24" s="9" t="s">
+        <v>97</v>
       </c>
       <c r="O24" s="2"/>
-      <c r="P24" s="15" t="s">
-        <v>97</v>
+      <c r="P24" s="17" t="s">
+        <v>98</v>
       </c>
       <c r="Q24" s="2"/>
-      <c r="R24" s="15"/>
+      <c r="R24" s="17"/>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
@@ -2166,19 +2158,19 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="7"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="9"/>
       <c r="M25" s="2"/>
-      <c r="N25" s="7" t="s">
-        <v>98</v>
+      <c r="N25" s="9" t="s">
+        <v>99</v>
       </c>
       <c r="O25" s="2"/>
-      <c r="P25" s="15" t="s">
-        <v>99</v>
+      <c r="P25" s="17" t="s">
+        <v>100</v>
       </c>
       <c r="Q25" s="2"/>
-      <c r="R25" s="15"/>
+      <c r="R25" s="17"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
@@ -2213,19 +2205,19 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="7"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="9"/>
       <c r="M26" s="2"/>
-      <c r="N26" s="7" t="s">
-        <v>100</v>
+      <c r="N26" s="9" t="s">
+        <v>101</v>
       </c>
       <c r="O26" s="2"/>
-      <c r="P26" s="15" t="s">
-        <v>101</v>
+      <c r="P26" s="17" t="s">
+        <v>102</v>
       </c>
       <c r="Q26" s="2"/>
-      <c r="R26" s="15"/>
+      <c r="R26" s="17"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
@@ -2260,19 +2252,19 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="7"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="9"/>
       <c r="M27" s="2"/>
-      <c r="N27" s="7" t="s">
-        <v>102</v>
+      <c r="N27" s="9" t="s">
+        <v>103</v>
       </c>
       <c r="O27" s="2"/>
-      <c r="P27" s="15" t="s">
-        <v>103</v>
+      <c r="P27" s="17" t="s">
+        <v>104</v>
       </c>
       <c r="Q27" s="2"/>
-      <c r="R27" s="15"/>
+      <c r="R27" s="17"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
@@ -2307,19 +2299,19 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="7"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="9"/>
       <c r="M28" s="2"/>
-      <c r="N28" s="7" t="s">
-        <v>104</v>
+      <c r="N28" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="O28" s="2"/>
-      <c r="P28" s="15" t="s">
-        <v>105</v>
+      <c r="P28" s="17" t="s">
+        <v>106</v>
       </c>
       <c r="Q28" s="2"/>
-      <c r="R28" s="15"/>
+      <c r="R28" s="17"/>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
@@ -2354,15 +2346,15 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="7"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="9"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
-      <c r="P29" s="15"/>
+      <c r="P29" s="17"/>
       <c r="Q29" s="2"/>
-      <c r="R29" s="15"/>
+      <c r="R29" s="17"/>
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
@@ -2397,15 +2389,15 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="7"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="9"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
-      <c r="P30" s="15"/>
+      <c r="P30" s="17"/>
       <c r="Q30" s="2"/>
-      <c r="R30" s="15"/>
+      <c r="R30" s="17"/>
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
@@ -2440,9 +2432,9 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="7"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="9"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -2483,9 +2475,9 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="7"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="9"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -2526,14 +2518,14 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="6" t="s">
-        <v>106</v>
+      <c r="J33" s="3"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="8" t="s">
+        <v>107</v>
       </c>
       <c r="M33" s="2"/>
-      <c r="N33" s="7" t="s">
-        <v>107</v>
+      <c r="N33" s="9" t="s">
+        <v>108</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
@@ -2573,12 +2565,12 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
+      <c r="J34" s="3"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
-      <c r="N34" s="7" t="s">
-        <v>108</v>
+      <c r="N34" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
@@ -2618,12 +2610,12 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
+      <c r="J35" s="3"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
-      <c r="N35" s="7" t="s">
-        <v>109</v>
+      <c r="N35" s="9" t="s">
+        <v>110</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
@@ -2663,7 +2655,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
+      <c r="J36" s="3"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
@@ -2706,8 +2698,8 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="6" t="s">
-        <v>110</v>
+      <c r="J37" s="8" t="s">
+        <v>111</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -2751,9 +2743,9 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="6" t="s">
-        <v>111</v>
+      <c r="J38" s="3"/>
+      <c r="K38" s="8" t="s">
+        <v>112</v>
       </c>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
@@ -2796,14 +2788,14 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
+      <c r="J39" s="3"/>
       <c r="K39" s="2"/>
-      <c r="L39" s="6" t="s">
-        <v>81</v>
+      <c r="L39" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="M39" s="2"/>
-      <c r="N39" s="7" t="s">
-        <v>112</v>
+      <c r="N39" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
@@ -2843,12 +2835,12 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
+      <c r="J40" s="3"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
-      <c r="N40" s="7" t="s">
-        <v>113</v>
+      <c r="N40" s="9" t="s">
+        <v>114</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
@@ -2888,14 +2880,14 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
+      <c r="J41" s="3"/>
       <c r="K41" s="2"/>
-      <c r="L41" s="6" t="s">
-        <v>114</v>
+      <c r="L41" s="8" t="s">
+        <v>115</v>
       </c>
       <c r="M41" s="2"/>
-      <c r="N41" s="7" t="s">
-        <v>115</v>
+      <c r="N41" s="9" t="s">
+        <v>116</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
@@ -2935,7 +2927,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
+      <c r="J42" s="3"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
@@ -2978,13 +2970,13 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L43" s="7"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="L43" s="9"/>
       <c r="M43" s="2"/>
-      <c r="N43" s="19"/>
+      <c r="N43" s="21"/>
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
@@ -3023,17 +3015,17 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="M44" s="7"/>
-      <c r="N44" s="7" t="s">
+      <c r="J44" s="3"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="O44" s="7" t="s">
+      <c r="M44" s="9"/>
+      <c r="N44" s="9" t="s">
         <v>83</v>
+      </c>
+      <c r="O44" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
@@ -3072,12 +3064,12 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
+      <c r="J45" s="3"/>
       <c r="K45" s="2"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
-      <c r="N45" s="7" t="s">
-        <v>117</v>
+      <c r="L45" s="9"/>
+      <c r="M45" s="9"/>
+      <c r="N45" s="9" t="s">
+        <v>118</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
@@ -3117,10 +3109,10 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
+      <c r="J46" s="3"/>
       <c r="K46" s="2"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
@@ -3160,22 +3152,22 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
+      <c r="J47" s="3"/>
       <c r="K47" s="2"/>
-      <c r="L47" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="M47" s="7"/>
-      <c r="N47" s="7" t="s">
+      <c r="L47" s="8" t="s">
         <v>92</v>
       </c>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9" t="s">
+        <v>93</v>
+      </c>
       <c r="O47" s="2"/>
-      <c r="P47" s="15" t="s">
-        <v>93</v>
+      <c r="P47" s="17" t="s">
+        <v>94</v>
       </c>
       <c r="Q47" s="2"/>
-      <c r="R47" s="15" t="s">
-        <v>118</v>
+      <c r="R47" s="17" t="s">
+        <v>119</v>
       </c>
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
@@ -3211,20 +3203,20 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
+      <c r="J48" s="3"/>
       <c r="K48" s="2"/>
-      <c r="L48" s="7"/>
-      <c r="M48" s="7"/>
-      <c r="N48" s="7" t="s">
-        <v>94</v>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="O48" s="2"/>
-      <c r="P48" s="15" t="s">
-        <v>95</v>
+      <c r="P48" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="Q48" s="2"/>
-      <c r="R48" s="15" t="s">
-        <v>119</v>
+      <c r="R48" s="17" t="s">
+        <v>120</v>
       </c>
       <c r="S48" s="2"/>
       <c r="T48" s="2"/>
@@ -3260,20 +3252,20 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
+      <c r="J49" s="3"/>
       <c r="K49" s="2"/>
-      <c r="L49" s="7"/>
-      <c r="M49" s="7"/>
-      <c r="N49" s="7" t="s">
-        <v>96</v>
+      <c r="L49" s="9"/>
+      <c r="M49" s="9"/>
+      <c r="N49" s="9" t="s">
+        <v>97</v>
       </c>
       <c r="O49" s="2"/>
-      <c r="P49" s="15" t="s">
-        <v>97</v>
+      <c r="P49" s="17" t="s">
+        <v>98</v>
       </c>
       <c r="Q49" s="2"/>
-      <c r="R49" s="15" t="s">
-        <v>120</v>
+      <c r="R49" s="17" t="s">
+        <v>121</v>
       </c>
       <c r="S49" s="2"/>
       <c r="T49" s="2"/>
@@ -3309,20 +3301,20 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
+      <c r="J50" s="3"/>
       <c r="K50" s="2"/>
-      <c r="L50" s="7"/>
-      <c r="M50" s="7"/>
-      <c r="N50" s="7" t="s">
-        <v>121</v>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9" t="s">
+        <v>122</v>
       </c>
       <c r="O50" s="2"/>
-      <c r="P50" s="15" t="s">
-        <v>99</v>
+      <c r="P50" s="17" t="s">
+        <v>100</v>
       </c>
       <c r="Q50" s="2"/>
-      <c r="R50" s="15" t="s">
-        <v>119</v>
+      <c r="R50" s="17" t="s">
+        <v>120</v>
       </c>
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
@@ -3358,20 +3350,20 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
+      <c r="J51" s="3"/>
       <c r="K51" s="2"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
-      <c r="N51" s="7" t="s">
-        <v>100</v>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="9" t="s">
+        <v>101</v>
       </c>
       <c r="O51" s="2"/>
-      <c r="P51" s="15" t="s">
-        <v>101</v>
+      <c r="P51" s="17" t="s">
+        <v>102</v>
       </c>
       <c r="Q51" s="2"/>
-      <c r="R51" s="15" t="s">
-        <v>119</v>
+      <c r="R51" s="17" t="s">
+        <v>120</v>
       </c>
       <c r="S51" s="2"/>
       <c r="T51" s="2"/>
@@ -3407,20 +3399,20 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
+      <c r="J52" s="3"/>
       <c r="K52" s="2"/>
-      <c r="L52" s="7"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="O52" s="20"/>
-      <c r="P52" s="21" t="s">
+      <c r="L52" s="9"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="Q52" s="20"/>
-      <c r="R52" s="21" t="s">
-        <v>119</v>
+      <c r="O52" s="9"/>
+      <c r="P52" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q52" s="9"/>
+      <c r="R52" s="17" t="s">
+        <v>120</v>
       </c>
       <c r="S52" s="2"/>
       <c r="T52" s="2"/>
@@ -3456,20 +3448,20 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
+      <c r="J53" s="3"/>
       <c r="K53" s="2"/>
-      <c r="L53" s="7"/>
-      <c r="M53" s="7"/>
-      <c r="N53" s="7" t="s">
-        <v>104</v>
+      <c r="L53" s="9"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="O53" s="2"/>
-      <c r="P53" s="15" t="s">
-        <v>122</v>
+      <c r="P53" s="17" t="s">
+        <v>123</v>
       </c>
       <c r="Q53" s="2"/>
-      <c r="R53" s="15" t="s">
-        <v>123</v>
+      <c r="R53" s="17" t="s">
+        <v>124</v>
       </c>
       <c r="S53" s="2"/>
       <c r="T53" s="2"/>
@@ -3505,10 +3497,10 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
+      <c r="J54" s="3"/>
       <c r="K54" s="2"/>
-      <c r="L54" s="7"/>
-      <c r="M54" s="7"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
@@ -3548,14 +3540,14 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
+      <c r="J55" s="3"/>
       <c r="K55" s="2"/>
-      <c r="L55" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="M55" s="7"/>
-      <c r="N55" s="7" t="s">
-        <v>124</v>
+      <c r="L55" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9" t="s">
+        <v>125</v>
       </c>
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
@@ -3595,12 +3587,12 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
+      <c r="J56" s="3"/>
       <c r="K56" s="2"/>
-      <c r="L56" s="7"/>
-      <c r="M56" s="7"/>
-      <c r="N56" s="7" t="s">
-        <v>125</v>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
@@ -3640,12 +3632,12 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
+      <c r="J57" s="3"/>
       <c r="K57" s="2"/>
-      <c r="L57" s="7"/>
-      <c r="M57" s="7"/>
-      <c r="N57" s="7" t="s">
-        <v>108</v>
+      <c r="L57" s="9"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
@@ -3685,12 +3677,12 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
+      <c r="J58" s="3"/>
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
-      <c r="N58" s="7" t="s">
-        <v>109</v>
+      <c r="N58" s="9" t="s">
+        <v>110</v>
       </c>
       <c r="O58" s="2"/>
       <c r="P58" s="2"/>
@@ -3730,7 +3722,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
+      <c r="J59" s="3"/>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
@@ -3773,8 +3765,8 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
-      <c r="J60" s="6" t="s">
-        <v>126</v>
+      <c r="J60" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
@@ -3818,9 +3810,9 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="6" t="s">
-        <v>127</v>
+      <c r="J61" s="3"/>
+      <c r="K61" s="8" t="s">
+        <v>128</v>
       </c>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
@@ -3863,14 +3855,14 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
+      <c r="J62" s="3"/>
       <c r="K62" s="2"/>
-      <c r="L62" s="6" t="s">
-        <v>81</v>
+      <c r="L62" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="M62" s="2"/>
-      <c r="N62" s="7" t="s">
-        <v>33</v>
+      <c r="N62" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
@@ -3910,12 +3902,12 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
+      <c r="J63" s="3"/>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
-      <c r="N63" s="7" t="s">
-        <v>124</v>
+      <c r="N63" s="9" t="s">
+        <v>125</v>
       </c>
       <c r="O63" s="2"/>
       <c r="P63" s="2"/>
@@ -3955,12 +3947,12 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
+      <c r="J64" s="3"/>
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
-      <c r="N64" s="7" t="s">
-        <v>128</v>
+      <c r="N64" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="O64" s="2"/>
       <c r="P64" s="2"/>
@@ -4000,7 +3992,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
+      <c r="J65" s="3"/>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
@@ -4043,8 +4035,8 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
-      <c r="J66" s="6" t="s">
-        <v>129</v>
+      <c r="J66" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
@@ -4097,14 +4089,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="4.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="16.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="6.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="4.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="16.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -4118,80 +4110,80 @@
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4200,12 +4192,12 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4216,24 +4208,24 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -4244,10 +4236,10 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="5" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix key id card make react rerender unexpectedly
</commit_message>
<xml_diff>
--- a/Usecase.xlsx
+++ b/Usecase.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="132">
   <si>
     <t>Localstorage</t>
   </si>
@@ -35,7 +35,10 @@
     <t>PK</t>
   </si>
   <si>
-    <t>ddmmyyyy</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>count++</t>
   </si>
   <si>
     <t>plan</t>
@@ -415,7 +418,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,6 +432,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Bellota"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -554,13 +563,13 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -569,46 +578,46 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="17" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="17" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -962,9 +971,9 @@
     <col min="41" max="41" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
       <c r="A1" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1007,34 +1016,34 @@
       <c r="AN1" s="2"/>
       <c r="AO1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21">
       <c r="A2" s="2"/>
       <c r="B2" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="3"/>
       <c r="K2" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O2" s="2"/>
       <c r="P2" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -1062,7 +1071,7 @@
       <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="21">
       <c r="A3" s="10"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1105,9 +1114,9 @@
       <c r="AN3" s="13"/>
       <c r="AO3" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21.75">
       <c r="A4" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1118,7 +1127,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="15"/>
       <c r="J4" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -1133,7 +1142,7 @@
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
@@ -1154,10 +1163,10 @@
       <c r="AN4" s="2"/>
       <c r="AO4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="21">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1167,12 +1176,12 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -1184,11 +1193,11 @@
       <c r="U5" s="16"/>
       <c r="V5" s="16"/>
       <c r="W5" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X5" s="2"/>
       <c r="Y5" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
@@ -1207,11 +1216,11 @@
       <c r="AN5" s="2"/>
       <c r="AO5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="21">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1221,21 +1230,21 @@
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
       <c r="K6" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
@@ -1243,7 +1252,7 @@
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
@@ -1264,11 +1273,11 @@
       <c r="AN6" s="2"/>
       <c r="AO6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="21">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1278,7 +1287,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
       <c r="K7" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -1292,11 +1301,11 @@
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="X7" s="2"/>
       <c r="Y7" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
@@ -1315,11 +1324,11 @@
       <c r="AN7" s="2"/>
       <c r="AO7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="21">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1330,19 +1339,19 @@
       <c r="J8" s="8"/>
       <c r="K8" s="2"/>
       <c r="L8" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="S8" s="8"/>
       <c r="T8" s="2"/>
@@ -1368,7 +1377,7 @@
       <c r="AN8" s="2"/>
       <c r="AO8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="21">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1381,19 +1390,19 @@
       <c r="J9" s="3"/>
       <c r="K9" s="2"/>
       <c r="L9" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
@@ -1419,10 +1428,10 @@
       <c r="AN9" s="2"/>
       <c r="AO9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="21">
       <c r="A10" s="2"/>
       <c r="B10" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1434,15 +1443,15 @@
       <c r="J10" s="3"/>
       <c r="K10" s="2"/>
       <c r="L10" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="19"/>
@@ -1470,11 +1479,11 @@
       <c r="AN10" s="2"/>
       <c r="AO10" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="21">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1485,13 +1494,13 @@
       <c r="J11" s="3"/>
       <c r="K11" s="2"/>
       <c r="L11" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
@@ -1519,7 +1528,7 @@
       <c r="AN11" s="2"/>
       <c r="AO11" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="21">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1533,10 +1542,10 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
@@ -1547,7 +1556,7 @@
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
       <c r="W12" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
@@ -1568,7 +1577,7 @@
       <c r="AN12" s="2"/>
       <c r="AO12" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="21">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1582,10 +1591,10 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
@@ -1596,11 +1605,11 @@
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="X13" s="2"/>
       <c r="Y13" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
@@ -1619,7 +1628,7 @@
       <c r="AN13" s="2"/>
       <c r="AO13" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="21">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1632,11 +1641,11 @@
       <c r="J14" s="3"/>
       <c r="K14" s="2"/>
       <c r="L14" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
@@ -1647,19 +1656,19 @@
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="X14" s="2"/>
       <c r="Y14" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Z14" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AD14" s="2"/>
       <c r="AE14" s="2"/>
@@ -1674,7 +1683,7 @@
       <c r="AN14" s="2"/>
       <c r="AO14" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="21">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1698,11 +1707,11 @@
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X15" s="2"/>
       <c r="Y15" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
@@ -1721,7 +1730,7 @@
       <c r="AN15" s="2"/>
       <c r="AO15" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="21">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1733,7 +1742,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="3"/>
       <c r="K16" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="2"/>
@@ -1747,11 +1756,11 @@
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
       <c r="W16" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="X16" s="2"/>
       <c r="Y16" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
@@ -1770,7 +1779,7 @@
       <c r="AN16" s="2"/>
       <c r="AO16" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="21">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1783,14 +1792,14 @@
       <c r="J17" s="3"/>
       <c r="K17" s="9"/>
       <c r="L17" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
@@ -1800,11 +1809,11 @@
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
       <c r="W17" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="X17" s="2"/>
       <c r="Y17" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
@@ -1823,7 +1832,7 @@
       <c r="AN17" s="2"/>
       <c r="AO17" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="21">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1838,7 +1847,7 @@
       <c r="L18" s="9"/>
       <c r="M18" s="2"/>
       <c r="N18" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
@@ -1849,11 +1858,11 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="X18" s="2"/>
       <c r="Y18" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
@@ -1872,7 +1881,7 @@
       <c r="AN18" s="2"/>
       <c r="AO18" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="21">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1915,7 +1924,7 @@
       <c r="AN19" s="2"/>
       <c r="AO19" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="21">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1939,11 +1948,11 @@
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
       <c r="W20" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="X20" s="2"/>
       <c r="Y20" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
@@ -1962,7 +1971,7 @@
       <c r="AN20" s="2"/>
       <c r="AO20" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="21">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2005,7 +2014,7 @@
       <c r="AN21" s="2"/>
       <c r="AO21" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="21">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2018,15 +2027,15 @@
       <c r="J22" s="3"/>
       <c r="K22" s="20"/>
       <c r="L22" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="17"/>
@@ -2054,7 +2063,7 @@
       <c r="AN22" s="2"/>
       <c r="AO22" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="21">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2069,11 +2078,11 @@
       <c r="L23" s="9"/>
       <c r="M23" s="2"/>
       <c r="N23" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="17"/>
@@ -2101,7 +2110,7 @@
       <c r="AN23" s="2"/>
       <c r="AO23" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="21">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2116,11 +2125,11 @@
       <c r="L24" s="9"/>
       <c r="M24" s="2"/>
       <c r="N24" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="17"/>
@@ -2148,7 +2157,7 @@
       <c r="AN24" s="2"/>
       <c r="AO24" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="21">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2163,11 +2172,11 @@
       <c r="L25" s="9"/>
       <c r="M25" s="2"/>
       <c r="N25" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="17"/>
@@ -2195,7 +2204,7 @@
       <c r="AN25" s="2"/>
       <c r="AO25" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="21">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2210,11 +2219,11 @@
       <c r="L26" s="9"/>
       <c r="M26" s="2"/>
       <c r="N26" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Q26" s="2"/>
       <c r="R26" s="17"/>
@@ -2242,7 +2251,7 @@
       <c r="AN26" s="2"/>
       <c r="AO26" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="21">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2257,11 +2266,11 @@
       <c r="L27" s="9"/>
       <c r="M27" s="2"/>
       <c r="N27" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q27" s="2"/>
       <c r="R27" s="17"/>
@@ -2289,7 +2298,7 @@
       <c r="AN27" s="2"/>
       <c r="AO27" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="21">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2304,11 +2313,11 @@
       <c r="L28" s="9"/>
       <c r="M28" s="2"/>
       <c r="N28" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" s="17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="Q28" s="2"/>
       <c r="R28" s="17"/>
@@ -2336,7 +2345,7 @@
       <c r="AN28" s="2"/>
       <c r="AO28" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="21">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2379,7 +2388,7 @@
       <c r="AN29" s="2"/>
       <c r="AO29" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="21">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2521,11 +2530,11 @@
       <c r="J33" s="3"/>
       <c r="K33" s="16"/>
       <c r="L33" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
@@ -2570,7 +2579,7 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
@@ -2615,7 +2624,7 @@
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
@@ -2699,7 +2708,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -2745,7 +2754,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="3"/>
       <c r="K38" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
@@ -2791,11 +2800,11 @@
       <c r="J39" s="3"/>
       <c r="K39" s="2"/>
       <c r="L39" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
@@ -2840,7 +2849,7 @@
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
@@ -2883,11 +2892,11 @@
       <c r="J41" s="3"/>
       <c r="K41" s="2"/>
       <c r="L41" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
@@ -2972,7 +2981,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="3"/>
       <c r="K43" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L43" s="9"/>
       <c r="M43" s="2"/>
@@ -3018,14 +3027,14 @@
       <c r="J44" s="3"/>
       <c r="K44" s="9"/>
       <c r="L44" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M44" s="9"/>
       <c r="N44" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O44" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
@@ -3069,7 +3078,7 @@
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
       <c r="N45" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
@@ -3155,19 +3164,19 @@
       <c r="J47" s="3"/>
       <c r="K47" s="2"/>
       <c r="L47" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M47" s="9"/>
       <c r="N47" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O47" s="2"/>
       <c r="P47" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Q47" s="2"/>
       <c r="R47" s="17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
@@ -3208,15 +3217,15 @@
       <c r="L48" s="9"/>
       <c r="M48" s="9"/>
       <c r="N48" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O48" s="2"/>
       <c r="P48" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Q48" s="2"/>
       <c r="R48" s="17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="S48" s="2"/>
       <c r="T48" s="2"/>
@@ -3257,15 +3266,15 @@
       <c r="L49" s="9"/>
       <c r="M49" s="9"/>
       <c r="N49" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O49" s="2"/>
       <c r="P49" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="Q49" s="2"/>
       <c r="R49" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="S49" s="2"/>
       <c r="T49" s="2"/>
@@ -3306,15 +3315,15 @@
       <c r="L50" s="9"/>
       <c r="M50" s="9"/>
       <c r="N50" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O50" s="2"/>
       <c r="P50" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Q50" s="2"/>
       <c r="R50" s="17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
@@ -3355,15 +3364,15 @@
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
       <c r="N51" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="O51" s="2"/>
       <c r="P51" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Q51" s="2"/>
       <c r="R51" s="17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="S51" s="2"/>
       <c r="T51" s="2"/>
@@ -3404,15 +3413,15 @@
       <c r="L52" s="9"/>
       <c r="M52" s="9"/>
       <c r="N52" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O52" s="9"/>
       <c r="P52" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q52" s="9"/>
       <c r="R52" s="17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="S52" s="2"/>
       <c r="T52" s="2"/>
@@ -3453,15 +3462,15 @@
       <c r="L53" s="9"/>
       <c r="M53" s="9"/>
       <c r="N53" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="Q53" s="2"/>
       <c r="R53" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="S53" s="2"/>
       <c r="T53" s="2"/>
@@ -3543,11 +3552,11 @@
       <c r="J55" s="3"/>
       <c r="K55" s="2"/>
       <c r="L55" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M55" s="9"/>
       <c r="N55" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
@@ -3592,7 +3601,7 @@
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
       <c r="N56" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
@@ -3637,7 +3646,7 @@
       <c r="L57" s="9"/>
       <c r="M57" s="9"/>
       <c r="N57" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
@@ -3682,7 +3691,7 @@
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="O58" s="2"/>
       <c r="P58" s="2"/>
@@ -3766,7 +3775,7 @@
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
@@ -3812,7 +3821,7 @@
       <c r="I61" s="2"/>
       <c r="J61" s="3"/>
       <c r="K61" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
@@ -3858,11 +3867,11 @@
       <c r="J62" s="3"/>
       <c r="K62" s="2"/>
       <c r="L62" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
@@ -3907,7 +3916,7 @@
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
       <c r="N63" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="O63" s="2"/>
       <c r="P63" s="2"/>
@@ -3952,7 +3961,7 @@
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
       <c r="N64" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O64" s="2"/>
       <c r="P64" s="2"/>
@@ -4036,7 +4045,7 @@
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
       <c r="J66" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
@@ -4128,63 +4137,65 @@
       <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="H2" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="2"/>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="2"/>
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="2"/>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
@@ -4195,10 +4206,10 @@
       <c r="E6" s="4"/>
       <c r="F6" s="2"/>
       <c r="G6" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
@@ -4209,10 +4220,10 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
@@ -4223,10 +4234,10 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
@@ -4237,10 +4248,10 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>